<commit_message>
update: requirement list & descriptions
</commit_message>
<xml_diff>
--- a/Requirement List.xlsx
+++ b/Requirement List.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwpark\Desktop\swe\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19395" windowHeight="9945"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="시트1" sheetId="1" r:id="rId4"/>
+    <sheet name="시트1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>No</t>
   </si>
@@ -56,30 +64,76 @@
   </si>
   <si>
     <t>대여 금액 및 횟수 통계</t>
+  </si>
+  <si>
+    <t>게스트가 필수 입력 정보 (ID, 비밀
+번호, 전화번호, 결제 수단, 선호 자전거 유형(일반/전기) 등)을 입력하여 회원 계정을 생성하는 기능</t>
+  </si>
+  <si>
+    <t>회원 가입</t>
+  </si>
+  <si>
+    <t>회원 정보를 회원 리스트에서 삭제하는 기능</t>
+  </si>
+  <si>
+    <t>회원 탈퇴</t>
+  </si>
+  <si>
+    <t>회원이 ID와 비밀번호를 입력하고 시스템에 접속한다.</t>
+  </si>
+  <si>
+    <t>로그인하기</t>
+  </si>
+  <si>
+    <t>로그아웃으로 시스템 접속을 종료한다.</t>
+  </si>
+  <si>
+    <t>로그아웃하기</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -93,46 +147,86 @@
         <bgColor rgb="FFF3F3F3"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3F3F3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
-    <border/>
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -322,25 +416,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="6.63"/>
-    <col customWidth="1" min="2" max="2" width="55.75"/>
-    <col customWidth="1" min="3" max="3" width="28.38"/>
+    <col min="1" max="1" width="6.5703125" customWidth="1"/>
+    <col min="2" max="2" width="55.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -351,9 +450,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -362,9 +461,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>5</v>
@@ -373,9 +472,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
@@ -384,9 +483,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>9</v>
@@ -395,9 +494,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>11</v>
@@ -406,9 +505,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>13</v>
@@ -417,7 +516,53 @@
         <v>14</v>
       </c>
     </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>